<commit_message>
added some examples of obtaining embeddings for bert model. Added another link to the important links
</commit_message>
<xml_diff>
--- a/meetings/important_links.xlsx
+++ b/meetings/important_links.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Link</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t xml:space="preserve">End-To-End Memory Networks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mccormickml.com/2019/05/14/BERT-word-embeddings-tutorial/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BERT Word Embeddings Tutorial</t>
   </si>
 </sst>
 </file>
@@ -53,11 +59,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -79,11 +86,27 @@
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="22"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,7 +151,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -138,6 +161,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -158,17 +189,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.7704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.0510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.7397959183674"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -203,11 +234,20 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="https://arxiv.org/pdf/1906.02916.pdf"/>
     <hyperlink ref="A3" r:id="rId2" display="https://arxiv.org/pdf/1911.10470.pdf"/>
     <hyperlink ref="A4" r:id="rId3" display="https://papers.nips.cc/paper/5846-end-to-end-memory-networks.pdf"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://mccormickml.com/2019/05/14/BERT-word-embeddings-tutorial/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>